<commit_message>
before update NgramSeqCount to do away with CoordTF (see NgramSeqCount2, reducing time to 1/30th of original
</commit_message>
<xml_diff>
--- a/notes/Q2 results vy coverage.xlsx
+++ b/notes/Q2 results vy coverage.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="120">
   <si>
     <t xml:space="preserve">case of the </t>
   </si>
@@ -306,6 +306,84 @@
   </si>
   <si>
     <t xml:space="preserve"> 567.59    0.08  567.67 </t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>ngram+word</t>
+  </si>
+  <si>
+    <t>ngram-model</t>
+  </si>
+  <si>
+    <t>[1] "of the"</t>
+  </si>
+  <si>
+    <t>[1] "the world"</t>
+  </si>
+  <si>
+    <t>[1] "the most"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.02    0.00    0.03 </t>
+  </si>
+  <si>
+    <t>[1] "the best" "the fact"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.01    0.00    0.01 </t>
+  </si>
+  <si>
+    <t>[1] "the end"</t>
+  </si>
+  <si>
+    <t>[1] "my way"</t>
+  </si>
+  <si>
+    <t>[1] "some time"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00    0.02    0.02 </t>
+  </si>
+  <si>
+    <t>[1] "little brother"</t>
+  </si>
+  <si>
+    <t>[1] "the day"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00    0.01    0.02 </t>
+  </si>
+  <si>
+    <t>[1] "be a"</t>
+  </si>
+  <si>
+    <t>[1] "case of the"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.03    0.01    0.05 </t>
+  </si>
+  <si>
+    <t>[1] "mean the world"</t>
+  </si>
+  <si>
+    <t>[1] "me the happiest"</t>
+  </si>
+  <si>
+    <t>character(0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.02    0.02    0.03 </t>
+  </si>
+  <si>
+    <t>[1] "on my way"</t>
+  </si>
+  <si>
+    <t>[1] "quite some time"</t>
+  </si>
+  <si>
+    <t>[1] "must be a"</t>
   </si>
 </sst>
 </file>
@@ -649,13 +727,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H46" sqref="H46"/>
+      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,1135 +742,1378 @@
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="5" width="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="8" width="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>3</v>
       </c>
-      <c r="C1">
+      <c r="C2">
         <v>3</v>
       </c>
-      <c r="D1">
+      <c r="D2">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="E2">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="F2">
         <v>4</v>
       </c>
-      <c r="G1">
+      <c r="G2">
         <v>4</v>
       </c>
-      <c r="H1">
+      <c r="H2">
         <v>4</v>
       </c>
-      <c r="I1" s="1">
+      <c r="I2" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>0.5</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>0.6</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>0.7</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>0.5</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>0.6</v>
       </c>
-      <c r="G2">
+      <c r="G3">
         <v>0.7</v>
       </c>
-      <c r="H2">
+      <c r="H3">
         <v>0.99</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I3" s="1">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="J3">
+        <v>0.5</v>
+      </c>
+      <c r="K3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="1">
+      <c r="J4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
         <v>497</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="1">
         <v>497</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D5" s="1">
         <v>497</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E5" s="1">
         <v>102</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F5" s="1">
         <v>102</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G5" s="1">
         <v>102</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H5" s="1">
         <v>102</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I5" s="1">
         <v>497</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="J7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
+      <c r="J8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
         <v>56923</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>300</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="1">
         <v>300</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E9" s="1">
         <v>56923</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F9" s="1">
         <v>201</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G9" s="1">
         <v>201</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H9" s="1">
         <v>201</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I9" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="J11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
+      <c r="J12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
         <v>284</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C13" s="1">
         <v>284</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D13" s="1">
         <v>284</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E13" s="1">
         <v>284</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F13" s="1">
         <v>284</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G13" s="1">
         <v>5</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H13" s="1">
         <v>28</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I13" s="1">
         <v>284</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="J15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="1">
+      <c r="J16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
         <v>228</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C17" s="1">
         <v>277</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D17" s="1">
         <v>277</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E17" s="1">
         <v>228</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F17" s="1">
         <v>277</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G17" s="1">
         <v>277</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H17" s="1">
         <v>277</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I17" s="1">
         <v>277</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="J19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="1">
+      <c r="J20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
         <v>5619</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C21" s="1">
         <v>8207</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D21" s="1">
         <v>8207</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E21" s="1">
         <v>5619</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F21" s="1">
         <v>8207</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G21" s="1">
         <v>8207</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H21" s="1">
         <v>2</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I21" s="1">
         <v>8207</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="J23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="1">
+      <c r="J24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
         <v>2348</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C25" s="1">
         <v>2348</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D25" s="1">
         <v>2348</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E25" s="1">
         <v>35</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F25" s="1">
         <v>35</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G25" s="1">
         <v>35</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H25" s="1">
         <v>35</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I25" s="1">
         <v>2348</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="J27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="1">
+      <c r="J28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
         <v>371</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C29" s="1">
         <v>371</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D29" s="1">
         <v>371</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E29" s="1">
         <v>43</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F29" s="1">
         <v>43</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G29" s="1">
         <v>43</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H29" s="1">
         <v>43</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I29" s="1">
         <v>371</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="J31" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="1">
+      <c r="J32" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
         <v>3515</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C33" s="1">
         <v>17</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D33" s="1">
         <v>33</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E33" s="1">
         <v>3515</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F33" s="1">
         <v>17</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G33" s="1">
         <v>33</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H33" s="1">
         <v>33</v>
       </c>
-      <c r="I32" s="1">
+      <c r="I33" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="J35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="1">
+      <c r="J36" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
         <v>951</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C37" s="1">
         <v>951</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D37" s="1">
         <v>951</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E37" s="1">
         <v>951</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F37" s="1">
         <v>951</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G37" s="1">
         <v>951</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H37" s="1">
         <v>951</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I37" s="1">
         <v>951</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="J39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="1">
+      <c r="J40" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
         <v>745</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C41" s="1">
         <v>745</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D41" s="1">
         <v>745</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E41" s="1">
         <v>93</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F41" s="1">
         <v>93</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G41" s="1">
         <v>93</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H41" s="1">
         <v>93</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I41" s="1">
         <v>745</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>83</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>